<commit_message>
This should have the box tracking 8/8/2025
</commit_message>
<xml_diff>
--- a/DataTracking.xlsx
+++ b/DataTracking.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminmakhlouf/Research_repos/Integrated_OtoShapeAnalysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwnetid-my.sharepoint.com/personal/ate89_uw_edu/Documents/Desktop/Otoliths/CW_OtoClassificationPhotos/Integrated_OtoShapeAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10E280CF-DC37-DB4E-A489-E8BDBF4D1270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{10E280CF-DC37-DB4E-A489-E8BDBF4D1270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A65A3714-E126-4EEE-98A7-11E421C3967A}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="740" windowWidth="24960" windowHeight="17260" xr2:uid="{2F849378-4E93-5442-B44C-BA5E3095B301}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{2F849378-4E93-5442-B44C-BA5E3095B301}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,9 +35,65 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="17">
+  <si>
+    <t>Oto Boxes Checked and Photographed (Non-broken and facing left)</t>
+  </si>
+  <si>
+    <t>Completed Boxes are Unhighlighted</t>
+  </si>
+  <si>
+    <t>Kusko:</t>
+  </si>
+  <si>
+    <t>1-100</t>
+  </si>
+  <si>
+    <t>101-200</t>
+  </si>
+  <si>
+    <t>201-300</t>
+  </si>
+  <si>
+    <t>301-400</t>
+  </si>
+  <si>
+    <t>401-500</t>
+  </si>
+  <si>
+    <t>501-600</t>
+  </si>
+  <si>
+    <t>Oto Count:</t>
+  </si>
+  <si>
+    <t>Initial:</t>
+  </si>
+  <si>
+    <t>New:</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>Yukon:</t>
+  </si>
+  <si>
+    <t>601-700</t>
+  </si>
+  <si>
+    <t>701-800</t>
+  </si>
+  <si>
+    <t>Nush:</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -45,13 +101,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -66,8 +157,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,12 +500,710 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22B080BF-E74F-B249-A554-49579AB593C1}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2019</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>2020</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>2021</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="2">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>2023</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" s="2">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>2024</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9" s="2">
+        <f>L7+L8</f>
+        <v>546</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>2016</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>2019</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>2020</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>2021</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" s="4"/>
+      <c r="K15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L15" s="4"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>2022</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L16" s="4">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>2023</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L17" s="4">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>2024</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L18" s="4">
+        <f>L16+L17</f>
+        <v>212</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>2015</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>2017</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>2019</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>2020</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>2021</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L25" s="6"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>2022</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L26" s="6">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L27" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>2024</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L28" s="6">
+        <f>L26+L27</f>
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>